<commit_message>
Improvements (developerfield, scaling), added tests
</commit_message>
<xml_diff>
--- a/src/main/resources/Profile.xlsx
+++ b/src/main/resources/Profile.xlsx
@@ -156,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8020" uniqueCount="4480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8024" uniqueCount="4480">
   <si>
     <t>Type Name</t>
   </si>
@@ -42734,8 +42734,8 @@
   <dimension ref="A1:P1349"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A930" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F945" sqref="F945"/>
+      <pane ySplit="1" topLeftCell="A938" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="F949" sqref="F949:J949"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57689,6 +57689,13 @@
       <c r="D945" s="8" t="s">
         <v>2092</v>
       </c>
+      <c r="F945" s="3"/>
+      <c r="G945"/>
+      <c r="H945"/>
+      <c r="I945" t="s">
+        <v>3721</v>
+      </c>
+      <c r="J945"/>
       <c r="P945" s="8">
         <v>1</v>
       </c>
@@ -57703,6 +57710,13 @@
       <c r="D946" s="8" t="s">
         <v>2092</v>
       </c>
+      <c r="F946" s="3"/>
+      <c r="G946"/>
+      <c r="H946"/>
+      <c r="I946" t="s">
+        <v>3721</v>
+      </c>
+      <c r="J946"/>
       <c r="P946" s="8">
         <v>1</v>
       </c>
@@ -57744,6 +57758,21 @@
       </c>
       <c r="D949" s="8" t="s">
         <v>47</v>
+      </c>
+      <c r="F949" s="3" t="s">
+        <v>3924</v>
+      </c>
+      <c r="G949">
+        <v>5</v>
+      </c>
+      <c r="H949">
+        <v>500</v>
+      </c>
+      <c r="I949" t="s">
+        <v>3572</v>
+      </c>
+      <c r="J949">
+        <v>16</v>
       </c>
       <c r="P949" s="8">
         <v>1</v>

</xml_diff>

<commit_message>
battery status message added to Global Profile
</commit_message>
<xml_diff>
--- a/src/main/resources/Profile.xlsx
+++ b/src/main/resources/Profile.xlsx
@@ -294,7 +294,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8060" uniqueCount="4485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8077" uniqueCount="4490">
   <si>
     <t>Type Name</t>
   </si>
@@ -13813,6 +13813,21 @@
   </si>
   <si>
     <t>On Edge830 is is the barometric altitude with correction based on GPS. This value is shown on display; first measurement: corrected_altitude=altitude</t>
+  </si>
+  <si>
+    <t>voltage</t>
+  </si>
+  <si>
+    <t>mV</t>
+  </si>
+  <si>
+    <t>mA</t>
+  </si>
+  <si>
+    <t>degC</t>
+  </si>
+  <si>
+    <t>Positive is charging, negative is discharging</t>
   </si>
 </sst>
 </file>
@@ -42882,8 +42897,8 @@
   <dimension ref="A1:P1338"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D583" sqref="D583:J583"/>
+      <pane ySplit="1" topLeftCell="A287" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C294" sqref="C294:D294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64104,16 +64119,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64162,6 +64178,14 @@
       </c>
       <c r="E3" s="3"/>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>1442</v>
+      </c>
+      <c r="D4">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -64169,10 +64193,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64305,9 +64332,7 @@
       <c r="M4" s="8"/>
       <c r="N4" s="9"/>
       <c r="O4" s="8"/>
-      <c r="P4" s="8">
-        <v>1</v>
-      </c>
+      <c r="P4" s="8"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
@@ -64331,9 +64356,7 @@
       <c r="M5" s="8"/>
       <c r="N5" s="9"/>
       <c r="O5" s="8"/>
-      <c r="P5" s="8">
-        <v>7</v>
-      </c>
+      <c r="P5" s="8"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
@@ -64356,9 +64379,7 @@
       <c r="M6" s="8"/>
       <c r="N6" s="9"/>
       <c r="O6" s="8"/>
-      <c r="P6" s="8">
-        <v>1</v>
-      </c>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
@@ -64381,9 +64402,7 @@
       <c r="M7" s="8"/>
       <c r="N7" s="9"/>
       <c r="O7" s="8"/>
-      <c r="P7" s="8">
-        <v>1</v>
-      </c>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
@@ -64407,9 +64426,7 @@
       <c r="M8" s="8"/>
       <c r="N8" s="9"/>
       <c r="O8" s="8"/>
-      <c r="P8" s="8">
-        <v>1</v>
-      </c>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
@@ -64433,9 +64450,7 @@
       <c r="M9" s="8"/>
       <c r="N9" s="9"/>
       <c r="O9" s="8"/>
-      <c r="P9" s="8">
-        <v>1</v>
-      </c>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
@@ -64469,9 +64484,7 @@
       <c r="M10" s="8"/>
       <c r="N10" s="9"/>
       <c r="O10" s="8"/>
-      <c r="P10" s="8">
-        <v>1</v>
-      </c>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
@@ -64495,9 +64508,7 @@
       <c r="M11" s="8"/>
       <c r="N11" s="9"/>
       <c r="O11" s="8"/>
-      <c r="P11" s="8">
-        <v>1</v>
-      </c>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
@@ -64521,9 +64532,7 @@
       <c r="M12" s="8"/>
       <c r="N12" s="9"/>
       <c r="O12" s="8"/>
-      <c r="P12" s="8">
-        <v>7</v>
-      </c>
+      <c r="P12" s="8"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -64577,8 +64586,100 @@
         <v>4480</v>
       </c>
     </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>253</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>3494</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4485</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+      <c r="I20" t="s">
+        <v>4486</v>
+      </c>
+      <c r="P20">
+        <v>4260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1573</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2091</v>
+      </c>
+      <c r="I21" t="s">
+        <v>4487</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>4489</v>
+      </c>
+      <c r="P21">
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>711</v>
+      </c>
+      <c r="D22" t="s">
+        <v>134</v>
+      </c>
+      <c r="I22" t="s">
+        <v>3605</v>
+      </c>
+      <c r="P22">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2030</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2090</v>
+      </c>
+      <c r="I23" t="s">
+        <v>4488</v>
+      </c>
+      <c r="P23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed error, added test
</commit_message>
<xml_diff>
--- a/src/main/resources/Profile.xlsx
+++ b/src/main/resources/Profile.xlsx
@@ -71454,7 +71454,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -71532,7 +71532,7 @@
         <v>4985</v>
       </c>
       <c r="D8">
-        <v>3886</v>
+        <v>3866</v>
       </c>
     </row>
   </sheetData>

</xml_diff>